<commit_message>
Refactor import and export feature
</commit_message>
<xml_diff>
--- a/TestImportAndExport/students.xlsx
+++ b/TestImportAndExport/students.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8555"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SinhVien" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>student_id</t>
   </si>
@@ -44,15 +44,6 @@
     <t>academic_year</t>
   </si>
   <si>
-    <t>permanent_address</t>
-  </si>
-  <si>
-    <t>temporary_address</t>
-  </si>
-  <si>
-    <t>mailing_address</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -71,10 +62,112 @@
     <t>student_status</t>
   </si>
   <si>
-    <t>Hoàng Anh Thương</t>
-  </si>
-  <si>
-    <t>2002-12-23</t>
+    <t>permanentAddress</t>
+  </si>
+  <si>
+    <t>temporaryAddress</t>
+  </si>
+  <si>
+    <t>mailingAddress</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>id_number</t>
+  </si>
+  <si>
+    <t>issue_date</t>
+  </si>
+  <si>
+    <t>expiry_date</t>
+  </si>
+  <si>
+    <t>issue_place</t>
+  </si>
+  <si>
+    <t>has_chip</t>
+  </si>
+  <si>
+    <t>issue_country</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Đinh Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>2019-2023</t>
+  </si>
+  <si>
+    <t>dha@gmail.com</t>
+  </si>
+  <si>
+    <t>0929302020</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Khoa Luật</t>
+  </si>
+  <si>
+    <t>Đại trà</t>
+  </si>
+  <si>
+    <t>Đã thôi học</t>
+  </si>
+  <si>
+    <t>9 Võ Thị Sáu, Phường 2, Quận Bình Thạnh, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>12 Hoàng Hoa Thám, Phường 5, Quận Phú Nhuận, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>CMND</t>
+  </si>
+  <si>
+    <t>778206393122</t>
+  </si>
+  <si>
+    <t>TP Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Trần Anh Hoàng</t>
+  </si>
+  <si>
+    <t>2020-2024</t>
+  </si>
+  <si>
+    <t>tah@gmail.com</t>
+  </si>
+  <si>
+    <t>0923228640</t>
+  </si>
+  <si>
+    <t>Khoa Tiếng Nhật</t>
+  </si>
+  <si>
+    <t>Đã tốt nghiệp</t>
+  </si>
+  <si>
+    <t>7 Nguyễn Văn Lượng, Phường 1, Quận Gò Vấp, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>20 Quang Trung, Phường 6, Quận Tân Phú, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>CCCD</t>
+  </si>
+  <si>
+    <t>012932897301</t>
+  </si>
+  <si>
+    <t>Thái Thương Hồng</t>
   </si>
   <si>
     <t>Nữ</t>
@@ -83,49 +176,73 @@
     <t>2022-2026</t>
   </si>
   <si>
-    <t>456 Lê Lợi, Phường 10, Quận Gò vấp, TP Hồ Chí Minh, Vietnam</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>111 Hùng Vương, Phường 3, Quận 9, TP Hồ Chí Minh, Vietnam</t>
-  </si>
-  <si>
-    <t>hat@gmail.com</t>
-  </si>
-  <si>
-    <t>0929388721</t>
-  </si>
-  <si>
-    <t>Vietnam</t>
-  </si>
-  <si>
-    <t>Khoa Tiếng Anh thương mại</t>
-  </si>
-  <si>
-    <t>Đề án</t>
+    <t>tth@gmail.com</t>
+  </si>
+  <si>
+    <t>0912738221</t>
+  </si>
+  <si>
+    <t>Khoa Tiếng Pháp</t>
   </si>
   <si>
     <t>Đang học</t>
   </si>
   <si>
-    <t>Phạm Thiên An</t>
-  </si>
-  <si>
-    <t>2002-09-13</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>2020-2024</t>
-  </si>
-  <si>
-    <t>pta@gmail.com</t>
-  </si>
-  <si>
-    <t>0912348721</t>
+    <t>44 Phan CHân Trinh, Phường 3, Quận 2, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>12 Nguyễn Văn Cừ, Phường 5, Quận 1, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>passport</t>
+  </si>
+  <si>
+    <t>p987629321</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Hộ chiếu phổ thông</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Khương</t>
+  </si>
+  <si>
+    <t>ntk@gmail.com</t>
+  </si>
+  <si>
+    <t>0999862182</t>
+  </si>
+  <si>
+    <t>Khoa công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>102 Dương Quảng Hàm, Phường 2, Quận 7, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>13 Nguyễn Trãi, Phường 5, Quận Phú Nhuận, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>012297406301</t>
+  </si>
+  <si>
+    <t>Đinh Hải Hoàng</t>
+  </si>
+  <si>
+    <t>dhh@gmail.com</t>
+  </si>
+  <si>
+    <t>0922937122</t>
+  </si>
+  <si>
+    <t>702 Điện Biên Phủ, Phường 4, Quận Gò Vấp, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>24 Nguyễn Trãi, Phường 5, Quận Phú Nhuận, TP Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>012203988301</t>
   </si>
 </sst>
 </file>
@@ -149,24 +266,24 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,28 +718,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -748,8 +865,9 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1133,18 +1251,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="19.1" customWidth="1"/>
+    <col min="3" max="3" width="10.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1187,104 +1307,343 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19">
       <c r="A2">
-        <v>22120007</v>
+        <v>19120007</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>37036</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>43700</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45590</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>20120011</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1">
+        <v>37519</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3"/>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>44829</v>
+      </c>
+      <c r="R3" s="1">
+        <v>47751</v>
+      </c>
+      <c r="S3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>20120008</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:22">
+      <c r="A4">
+        <v>22120014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1">
+        <v>38268</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>44903</v>
+      </c>
+      <c r="R4" s="1">
+        <v>48380</v>
+      </c>
+      <c r="S4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>22120015</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1">
+        <v>38038</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>44696</v>
+      </c>
+      <c r="R5" s="1">
+        <v>47751</v>
+      </c>
+      <c r="S5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>22120016</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1">
+        <v>38219</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J6" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>44829</v>
+      </c>
+      <c r="R6" s="1">
+        <v>47751</v>
+      </c>
+      <c r="S6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="hat@gmail.com" tooltip="mailto:hat@gmail.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="pta@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="dha@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="tah@gmail.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="tth@gmail.com"/>
+    <hyperlink ref="F5" r:id="rId4" display="ntk@gmail.com"/>
+    <hyperlink ref="F6" r:id="rId5" display="dhh@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C2 E2:H2 J2:N3 C3:H3 A1:N1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:V1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>